<commit_message>
few fixes and updates
</commit_message>
<xml_diff>
--- a/reporting/report_template.xlsx
+++ b/reporting/report_template.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\felix\Dev\xlwings-eikon\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75A65EB-658E-4A0F-ACC9-6F55484AF3BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06497795-95BF-49E7-B15B-575658F657C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{2269DA39-2FA8-EE4B-884F-E4AE05C32F51}"/>
+    <workbookView xWindow="2730" yWindow="2160" windowWidth="17280" windowHeight="10073" xr2:uid="{2269DA39-2FA8-EE4B-884F-E4AE05C32F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
-    <sheet name="Config" sheetId="3" r:id="rId2"/>
-    <sheet name="Data" sheetId="2" r:id="rId3"/>
+    <sheet name="report_template.py" sheetId="4" r:id="rId2"/>
+    <sheet name="Config" sheetId="3" r:id="rId3"/>
+    <sheet name="Data" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="date_format">Config!$B$2</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>{{ perf_start_date }} - {{ perf_end_date }}</t>
   </si>
@@ -143,6 +144,201 @@
   <si>
     <t>&lt;frame&gt;</t>
   </si>
+  <si>
+    <t>import os</t>
+  </si>
+  <si>
+    <t>import datetime as dt</t>
+  </si>
+  <si>
+    <t>import numpy as np</t>
+  </si>
+  <si>
+    <t>import eikon as ek</t>
+  </si>
+  <si>
+    <t>import xlwings as xw</t>
+  </si>
+  <si>
+    <t># Requires a license key: https://www.xlwings.org/trial</t>
+  </si>
+  <si>
+    <t>from xlwings.pro.reports import create_report</t>
+  </si>
+  <si>
+    <t>def main():</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    template = xw.Book.caller()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Eikon setup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ek.set_app_key(os.getenv('EIKON_APP_KEY'))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Configuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    date_format = template.sheets['Config']['date_format'].value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if date_format == 'UK':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        fmt = '%e %b %Y'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    elif date_format == 'US':</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        fmt = '%b %e, %Y'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    else:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    instrument = template.sheets['Config']['instrument'].value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    start_date = dt.datetime(dt.datetime.now().year - 4, 1, 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Prices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    prices = ek.get_timeseries(instrument,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               fields=['close'],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               start_date=start_date,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               end_date=dt.datetime.now(),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               interval='weekly')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    end_date = prices.index[-1]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Summary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    summary, err = ek.get_data(instrument,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                               ['TR.PriceClose', 'TR.Volume', 'TR.PriceLow', 'TR.PriceHigh',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                'TR.IndexName', 'TR.IndexCalculationCurrency'])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Constituents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    constituents, err = ek.get_data(f'0#{instrument}',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    fields=['TR.CommonName', 'TR.PriceClose', 'TR.TotalReturnYTD'])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    constituents = constituents.set_index('Company Common Name')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Add empty columns so it goes into the desired Excel cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for i in range(6):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        constituents.insert(loc=i, column='merged' + str(i), value=np.nan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    constituents = constituents.drop(['Instrument'], axis=1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    constituents = constituents.rename(columns={"YTD Total Return": "YTD %"})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    constituents = constituents.sort_values("YTD %", ascending=False)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Collect data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    data = dict(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        perf_start_date=start_date.strftime(fmt),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        perf_end_date=end_date.strftime(fmt),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        index_name=summary.loc[0, 'Index Name'],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        currency=summary.loc[0, 'Calculation Currency'],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        reference_date=dt.date.today().strftime(fmt),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        historical_perf=prices,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        constituents=constituents,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        price_close=float(summary['Price Close']),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        volume=float(summary['Volume']),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        price_low=float(summary['Price Low']),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        price_high=float(summary['Price High'])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Create the Excel report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    app = template.app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    app.screen_updating = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wb = create_report(template.fullname,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       report_path, app=app, **data)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    app.screen_updating = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    wb.sheets.active["A1"].select()</t>
+  </si>
+  <si>
+    <t>from pathlib import Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    report_path = Path(template.fullname).resolve().parent / 'report.xlsx'</t>
+  </si>
 </sst>
 </file>
 
@@ -152,7 +348,7 @@
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,6 +404,12 @@
       <color theme="0"/>
       <name val="Avenir Book"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -268,7 +470,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -313,6 +515,8 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1554,6 +1758,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1567,9 +1772,10 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="33" x14ac:dyDescent="1.1499999999999999">
-      <c r="D3" s="19" t="s">
+      <c r="C3" s="19" t="s">
         <v>12</v>
       </c>
+      <c r="D3" s="1"/>
       <c r="E3" s="20"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
@@ -1584,7 +1790,8 @@
       <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="D4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1597,9 +1804,10 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="22.9" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
@@ -1612,6 +1820,7 @@
       <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -2117,6 +2326,392 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4908C1F3-B84A-48CC-8472-77BBBC342BD1}">
+  <dimension ref="A1:A79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="70.5625" style="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A1" s="27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A2" s="27" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A3" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A4" s="27"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A5" s="27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A6" s="27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A7" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A8" s="27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A9" s="27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A10" s="27"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A11" s="27"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A12" s="27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A13" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A14" s="27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A15" s="27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A16" s="27"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A17" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A18" s="27" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A19" s="27"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A20" s="27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A21" s="27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A22" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A23" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A24" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A25" s="27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A26" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A27" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A28" s="27"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A29" s="27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A30" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A31" s="27"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A32" s="27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A33" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A34" s="27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A35" s="27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A36" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A37" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A38" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A39" s="27"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A40" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A41" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A42" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A43" s="27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A44" s="27"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A45" s="27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A46" s="27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A47" s="27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A48" s="27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A49" s="27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A50" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A51" s="27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A52" s="27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A53" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A54" s="27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A55" s="27"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A56" s="27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A57" s="27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A58" s="27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A59" s="27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A60" s="27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A61" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A62" s="27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A63" s="27" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A64" s="27" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A65" s="27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A66" s="27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A67" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A68" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A69" s="27" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A70" s="27"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A71" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A72" s="27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A73" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A74" s="27"/>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A75" s="27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A76" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A77" s="27"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A78" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.5">
+      <c r="A79" s="27" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D9C90E-6834-4F4F-8885-2B2A155A9D2D}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -2165,7 +2760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C44023-5623-E647-83FE-FCAF22653932}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I2712"/>

</xml_diff>